<commit_message>
update application image :)
</commit_message>
<xml_diff>
--- a/Document/money.xlsx
+++ b/Document/money.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Chi phí</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Tổng chi</t>
+  </si>
+  <si>
+    <t>[SMAC] Venus</t>
   </si>
 </sst>
 </file>
@@ -528,7 +531,7 @@
   <dimension ref="A2:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -840,16 +843,11 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="G15" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="6">
-        <f>SUM(H3:H14)</f>
-        <v>7000</v>
-      </c>
-      <c r="I15" s="6">
-        <f>SUM(I3:I14)</f>
-        <v>0</v>
+      <c r="G15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="4">
+        <v>550</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -878,9 +876,17 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="G18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="6">
+        <f>SUM(H3:H15)</f>
+        <v>7550</v>
+      </c>
+      <c r="I18" s="6">
+        <f>SUM(I3:I14)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>

</xml_diff>